<commit_message>
new risk reg table as PDF
</commit_message>
<xml_diff>
--- a/Figures/RiskRegister.xlsx
+++ b/Figures/RiskRegister.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="aLIGO 42015" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'aLIGO 42015'!$A$1:$H$19</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -126,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -159,18 +161,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -182,12 +178,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -217,7 +207,7 @@
     </border>
   </borders>
   <cellStyleXfs count="9">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -227,41 +217,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,67 +587,67 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H19" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="6" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="14.5" style="6"/>
+    <col min="1" max="1" width="32.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="4">
         <v>75</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="7">
         <v>0.3</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="4">
         <v>10</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="6">
         <v>90</v>
       </c>
       <c r="H2" s="9">
@@ -678,25 +656,25 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="4">
         <v>60</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="7">
         <v>0.5</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="5">
         <v>18</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="4">
         <v>30</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="6">
         <v>50</v>
       </c>
       <c r="H3" s="9">
@@ -705,25 +683,25 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="4">
         <v>15</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="7">
         <v>0.1</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="6">
         <v>5</v>
       </c>
       <c r="H4" s="9">
@@ -732,25 +710,25 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="4">
         <v>25</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7">
         <v>0.03</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="4">
         <v>15</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="6">
         <v>15</v>
       </c>
       <c r="H5" s="9">
@@ -759,25 +737,25 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="4">
         <v>65</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <v>0.03</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="5">
         <v>6</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="6">
         <v>90</v>
       </c>
       <c r="H6" s="9">
@@ -786,25 +764,25 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="4">
         <v>33</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7">
         <v>0.15</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="4">
         <v>3</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="6">
         <v>65</v>
       </c>
       <c r="H7" s="9">
@@ -813,25 +791,25 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="4">
         <v>50</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="7">
         <v>0.5</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="5">
         <v>6</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="4">
         <v>40</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>5</v>
       </c>
       <c r="H8" s="9">
@@ -840,25 +818,25 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="4">
         <v>90</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="7">
         <v>0.35</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="5">
         <v>6</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="4">
         <v>33</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="6">
         <v>3</v>
       </c>
       <c r="H9" s="9">
@@ -867,25 +845,25 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="4">
         <v>50</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7">
         <v>0.2</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="5">
         <v>4</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="4">
         <v>15</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="6">
         <v>40</v>
       </c>
       <c r="H10" s="9">
@@ -894,25 +872,25 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="4">
         <v>70</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7">
         <v>0.2</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="5">
         <v>4</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="4">
         <v>40</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>5</v>
       </c>
       <c r="H11" s="9">
@@ -921,25 +899,25 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>25</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="7">
         <v>0.25</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="5">
         <v>7</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="6">
         <v>50</v>
       </c>
       <c r="H12" s="9">
@@ -948,25 +926,25 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>20</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="7">
         <v>0.75</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="5">
         <v>8</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="4">
         <v>30</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="6">
         <v>3</v>
       </c>
       <c r="H13" s="9">
@@ -975,25 +953,25 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="4">
         <v>55</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="7">
         <v>0.1</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="5">
         <v>3</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="4">
         <v>10</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="6">
         <v>2</v>
       </c>
       <c r="H14" s="9">
@@ -1002,25 +980,25 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="4">
         <v>70</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="7">
         <v>0.1</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="5">
         <v>2</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="4">
         <v>10</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="6">
         <v>3</v>
       </c>
       <c r="H15" s="9">
@@ -1029,25 +1007,25 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="4">
         <v>40</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="7">
         <v>0.6</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="5">
         <v>4</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="4">
         <v>30</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="6">
         <v>5</v>
       </c>
       <c r="H16" s="9">
@@ -1056,25 +1034,25 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="4">
         <v>80</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="7">
         <v>0.15</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="5">
         <v>3</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="4">
         <v>20</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="6">
         <v>95</v>
       </c>
       <c r="H17" s="9">
@@ -1083,25 +1061,25 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="4">
         <v>35</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="7">
         <v>0.15</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="4">
         <v>80</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="6">
         <v>10</v>
       </c>
       <c r="H18" s="9">
@@ -1110,25 +1088,25 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="4">
         <v>10</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="7">
         <v>0.03</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="4">
         <v>100</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="6">
         <v>100</v>
       </c>
       <c r="H19" s="9">
@@ -1196,21 +1174,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>